<commit_message>
add tasks positioning in time
</commit_message>
<xml_diff>
--- a/complete_schedule.xlsx
+++ b/complete_schedule.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mishin Danila\PycharmProjects\ScheduleApp\init_excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7155" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Schedule" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
@@ -24,42 +29,27 @@
   <si>
     <t>Deadline</t>
   </si>
-  <si>
-    <t>English Exam</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Math</t>
-  </si>
-  <si>
-    <t>600</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="204"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,17 +65,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -351,26 +350,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="21.7109375"/>
-    <col customWidth="1" max="2" min="2" width="21.85546875"/>
-    <col customWidth="1" max="3" min="3" width="19.7109375"/>
-    <col customWidth="1" max="4" min="4" width="12.42578125"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,30 +376,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="n"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>